<commit_message>
Add the support of note in vocabulary.
</commit_message>
<xml_diff>
--- a/data/animal.xlsx
+++ b/data/animal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ZZC/go/src/github.com/zzc-tongji/mydictionary-local-cli/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ZZC/go/src/github.com/zzc-tongji/mydictionary/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="animal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animal!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animal!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>SN</t>
   </si>
@@ -88,6 +88,15 @@
     <t>v. 承受；忍受；不适于某事（或做某事）；承担责任
 n. 熊；（在证券市场等）卖空的人
 网络 小熊；负担；容忍</t>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The cat sat in front of the bird cage in an agony of frustration at being so near and yet so far.
+猫无可奈何地坐在鸟笼前，眼看着鸟儿近在咫尺，可怎么也够不着。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -504,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -516,12 +525,13 @@
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="5"/>
+    <col min="4" max="4" width="60.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -532,13 +542,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -548,12 +561,15 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -563,12 +579,13 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -578,12 +595,13 @@
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4"/>
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -593,12 +611,13 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -608,13 +627,14 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:F1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>